<commit_message>
Allow for text formatting
</commit_message>
<xml_diff>
--- a/local-scenarios-new/cough/Scenario.xlsx
+++ b/local-scenarios-new/cough/Scenario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Process</t>
   </si>
@@ -28,52 +28,10 @@
     <t xml:space="preserve">Action</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUMP(B)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF [var] == few_days THEN JUMP(C) ELSE JUMP(D)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNLESS IS_LOADED(D) THEN JUMP(E) ELSE JUMP(D)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF [var] THEN JUMP(E) ELSE JUMP(F)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOR [i] IN [cart_items] DO LOAD(ExplainProduct WITH [i]); LOAD(K)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF IS_NEXT(G) THEN JUMP(H) ELSE JUMP(I)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF (IS_LOADED(H) OR [var2] == lol) THEN JUMP(J) ELSE JUMP(K)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF IS_NEXT(G) THEN (IF IS_LOADED(K) THEN JUMP(L) ELSE JUMP(M)) ELSE JUMP(I)</t>
+    <t xml:space="preserve">ExampleProcess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFER()</t>
   </si>
 </sst>
 </file>
@@ -252,14 +210,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="76.14"/>
   </cols>
   <sheetData>
@@ -277,62 +236,6 @@
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>